<commit_message>
Update ATD10b - Resultat før skat.xlsx
tilføjede String fejl
-Bille
</commit_message>
<xml_diff>
--- a/05 Test/ATD10b - Resultat før skat.xlsx
+++ b/05 Test/ATD10b - Resultat før skat.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ffadfded41a68b1b/Skrivebord/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruger\Documents\GitHub\HoeKulator\05 Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0759EDB9-B59C-4211-B066-5555F9C3F6EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7F25FB-B45E-43AC-9F3F-D4FDB55C2209}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E96B9F9D-9139-4AC8-8EC5-3427FAD41271}"/>
   </bookViews>
   <sheets>
     <sheet name="Testcases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -120,6 +120,18 @@
   </si>
   <si>
     <t>Resultat før skat</t>
+  </si>
+  <si>
+    <t>Resultat før renter = fem</t>
+  </si>
+  <si>
+    <t>Fejl forkerteDatatype resultatFørRenter = fem</t>
+  </si>
+  <si>
+    <t>Rente omkostninger = ti</t>
+  </si>
+  <si>
+    <t>Fejl forkerteDatatype renteOmkostninger = ti</t>
   </si>
 </sst>
 </file>
@@ -152,7 +164,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -247,15 +259,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -278,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -286,8 +289,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -298,7 +300,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -625,7 +627,7 @@
   <dimension ref="A2:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,25 +639,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
+      <c r="A2" s="15"/>
       <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="16"/>
+      <c r="A3" s="15"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>3</v>
       </c>
     </row>
@@ -676,10 +678,10 @@
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <v>150</v>
       </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
@@ -698,7 +700,7 @@
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <v>-300</v>
       </c>
       <c r="D8" s="2"/>
@@ -711,7 +713,7 @@
       <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -721,7 +723,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="8"/>
+      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
@@ -740,7 +742,7 @@
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="11">
         <v>1875</v>
       </c>
       <c r="D12" s="2"/>
@@ -753,7 +755,7 @@
       <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>21</v>
       </c>
     </row>
@@ -763,7 +765,7 @@
         <v>17</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="8"/>
+      <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
@@ -790,10 +792,10 @@
       <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>24</v>
       </c>
     </row>
@@ -802,10 +804,10 @@
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="13">
         <v>2500</v>
       </c>
-      <c r="D18" s="8"/>
+      <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
@@ -828,52 +830,68 @@
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="1"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="2"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
+      <c r="A23" s="3"/>
+      <c r="B23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="9"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="8"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>